<commit_message>
Add plain csv file
</commit_message>
<xml_diff>
--- a/BAT8266csv.xlsx
+++ b/BAT8266csv.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="BAT8266csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -429,7 +429,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -614,34 +614,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <left/>
+      <right style="thick">
         <color indexed="64"/>
       </right>
       <top/>
@@ -696,7 +670,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -723,8 +697,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1070,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W785"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,14 +1099,14 @@
         <v>-1.9047619047619063E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42422.727129629631</v>
       </c>
       <c r="B3">
         <v>1399</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="12">
         <v>4.2</v>
       </c>
       <c r="D3">
@@ -1711,7 +1683,7 @@
       <c r="U18" s="12"/>
       <c r="V18" s="13"/>
     </row>
-    <row r="19" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>42422.781006944446</v>
       </c>
@@ -1781,7 +1753,7 @@
       <c r="S20" s="12"/>
       <c r="T20" s="12"/>
       <c r="U20" s="12"/>
-      <c r="V20" s="19"/>
+      <c r="V20" s="13"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -1807,7 +1779,7 @@
         <v>17</v>
       </c>
       <c r="K21" s="12"/>
-      <c r="V21" s="20"/>
+      <c r="V21" s="13"/>
     </row>
     <row r="22" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -1843,7 +1815,7 @@
       <c r="S22" s="15"/>
       <c r="T22" s="15"/>
       <c r="U22" s="15"/>
-      <c r="V22" s="21"/>
+      <c r="V22" s="19"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="1">

</xml_diff>